<commit_message>
Added version 25 bug mapping
</commit_message>
<xml_diff>
--- a/bugs/25/bugs-source.xlsx
+++ b/bugs/25/bugs-source.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
   <si>
     <t>Bug ID</t>
   </si>
@@ -157,6 +157,77 @@
   </si>
   <si>
     <t>docker-1.12.6-3.git51ef5a8.fc25</t>
+  </si>
+  <si>
+    <t>Regression: Atomic DBus VulnerabilityInfo API hangs loading results from /var/lib/atomic</t>
+  </si>
+  <si>
+    <t>atomic-1.14.1-1.fc25.x86_64</t>
+  </si>
+  <si>
+    <t>java-1.8.0-openjdk: NSS 3.28 update causes core dump</t>
+  </si>
+  <si>
+    <t>java-1.8.0-openjdk-1.8.0.111-5.b16.fc25.x86_64</t>
+  </si>
+  <si>
+    <t>java.security</t>
+  </si>
+  <si>
+    <t>PHP doesn&amp;apos;t fallback to urandom when getrandom is not available</t>
+  </si>
+  <si>
+    <t>php-7.0.17-1.fc25</t>
+  </si>
+  <si>
+    <t>rpc.gssd fails to call into gssproxy</t>
+  </si>
+  <si>
+    <t>selinux-policy</t>
+  </si>
+  <si>
+    <t>rpc.gssd</t>
+  </si>
+  <si>
+    <t>CVE-2017-5428 firefox: Mozilla: integer overflow in createImageBitmap() (MFSA 2017-08)</t>
+  </si>
+  <si>
+    <t>firefox-52.0-6.fc25</t>
+  </si>
+  <si>
+    <t>createImageBitmap()</t>
+  </si>
+  <si>
+    <t>kexec: failed load kdump kernel - Can&amp;apos;t find kernel text map area from kcore</t>
+  </si>
+  <si>
+    <t>kernel-4.10.8-200.fc25.x86_64
+kexec-tools-2.0.13-7.fc25.1.x86_64</t>
+  </si>
+  <si>
+    <t>kernel.c</t>
+  </si>
+  <si>
+    <t>cjdroute and others fail to call sodium_init()</t>
+  </si>
+  <si>
+    <t>cjdns</t>
+  </si>
+  <si>
+    <t>contrib/c/privatetopublic.c 
+contrib/c/sybilsim.c 
+contrib/c/mkpasswd.c 
+contrib/c/makekeys.c 
+contrib/c/publictoip6.c 
+test/testcjdroute.c 
+crypto/random/randombytes.c 
+client/cjdroute2.c</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>NetworkManager GUI doesn&amp;apos;t allow for secure configuration of WPA(2) Enterprise networks (802.1x) [lr/tls-domain-suffix-match-rh1457542</t>
   </si>
 </sst>
 </file>
@@ -482,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,6 +867,213 @@
         <v>15</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1412189</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1414010</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1415137</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1427255</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1430963</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1433819</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1440587</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1455317</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1457542</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>